<commit_message>
fixed dumb overwrite bug
</commit_message>
<xml_diff>
--- a/school_schedule/media/data_model.xlsx
+++ b/school_schedule/media/data_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\Documents\personal_projects\school_schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{431508D2-BFDC-4829-946C-884FEC5025BB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D804198E-BE8A-412E-9100-CDE582AF6EBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{A8BC3741-A0C7-4FBD-9D2E-D02AE428C330}"/>
+    <workbookView xWindow="23610" yWindow="2865" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A8BC3741-A0C7-4FBD-9D2E-D02AE428C330}"/>
   </bookViews>
   <sheets>
     <sheet name="Availabilities" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB669183-54EE-4860-81E6-21DEA3055301}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -867,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB07282-9C3E-4F9E-978E-A53AF7929BA2}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
abstracted for franks model
</commit_message>
<xml_diff>
--- a/school_schedule/media/data_model.xlsx
+++ b/school_schedule/media/data_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\Documents\personal_projects\school_schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D804198E-BE8A-412E-9100-CDE582AF6EBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{431508D2-BFDC-4829-946C-884FEC5025BB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23610" yWindow="2865" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{A8BC3741-A0C7-4FBD-9D2E-D02AE428C330}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{A8BC3741-A0C7-4FBD-9D2E-D02AE428C330}"/>
   </bookViews>
   <sheets>
     <sheet name="Availabilities" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB669183-54EE-4860-81E6-21DEA3055301}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -867,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB07282-9C3E-4F9E-978E-A53AF7929BA2}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>